<commit_message>
Fix #4002 Model DAS-MODELv1.6.xlsx import error
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/DAS-MODELv1.6.xlsx
+++ b/molgenis-model-registry/src/test/resources/DAS-MODELv1.6.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31980" windowHeight="17320" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="17325" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="6" r:id="rId1"/>
@@ -1098,9 +1098,6 @@
     <t>testrange</t>
   </si>
   <si>
-    <t>coordinate string</t>
-  </si>
-  <si>
     <t>created</t>
   </si>
   <si>
@@ -1275,9 +1272,6 @@
   </si>
   <si>
     <t>orientation</t>
-  </si>
-  <si>
-    <t>subparts </t>
   </si>
   <si>
     <t>The tag content (optional) provides a human readable for display purposes. If omitted, it is assumed the ID is appropriate for display.</t>
@@ -1881,12 +1875,18 @@
   <si>
     <t>das_dasep_segment</t>
   </si>
+  <si>
+    <t>coordinate_string</t>
+  </si>
+  <si>
+    <t>subparts</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2970,167 +2970,7 @@
     <cellStyle name="Hyperlink" xfId="498" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="62">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="46">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3593,6 +3433,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3925,13 +3770,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.625" customWidth="1"/>
+    <col min="2" max="2" width="38.375" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.875" customWidth="1"/>
+    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3948,7 +3793,7 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3956,97 +3801,97 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B5" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B8" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -4068,9 +3913,9 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4093,7 +3938,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C2" t="s">
         <v>344</v>
@@ -4104,7 +3949,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C3" t="s">
         <v>345</v>
@@ -4115,21 +3960,21 @@
         <v>351</v>
       </c>
       <c r="B4" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4137,10 +3982,10 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4148,10 +3993,10 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4159,10 +4004,10 @@
         <v>347</v>
       </c>
       <c r="B8" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4170,10 +4015,10 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4181,186 +4026,186 @@
         <v>353</v>
       </c>
       <c r="B10" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>395</v>
+      </c>
+      <c r="B11" t="s">
+        <v>538</v>
+      </c>
+      <c r="C11" t="s">
         <v>396</v>
-      </c>
-      <c r="B11" t="s">
-        <v>540</v>
-      </c>
-      <c r="C11" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B12" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B13" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C13" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B14" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>418</v>
+      </c>
+      <c r="B15" t="s">
+        <v>539</v>
+      </c>
+      <c r="C15" t="s">
         <v>420</v>
-      </c>
-      <c r="B15" t="s">
-        <v>541</v>
-      </c>
-      <c r="C15" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B16" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C16" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B17" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B18" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C18" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B19" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C19" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B20" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C20" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B21" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C21" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B22" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C22" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B23" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C23" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B24" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C24" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B25" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C25" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B26" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C26" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -4368,21 +4213,21 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C27" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B28" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C28" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -4402,14 +4247,14 @@
   <dimension ref="A1:N104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.375" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.625" customWidth="1"/>
     <col min="4" max="4" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4454,7 +4299,7 @@
         <v>16</v>
       </c>
       <c r="N1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -4462,7 +4307,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -4482,7 +4327,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -4499,10 +4344,10 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B4" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -4514,7 +4359,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -4522,19 +4367,19 @@
         <v>347</v>
       </c>
       <c r="B5" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -4542,7 +4387,7 @@
         <v>348</v>
       </c>
       <c r="B6" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -4554,7 +4399,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -4562,7 +4407,7 @@
         <v>349</v>
       </c>
       <c r="B7" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -4571,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -4579,7 +4424,7 @@
         <v>350</v>
       </c>
       <c r="B8" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -4588,7 +4433,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -4596,7 +4441,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -4605,7 +4450,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -4613,19 +4458,19 @@
         <v>351</v>
       </c>
       <c r="B10" t="s">
+        <v>544</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>546</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>548</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -4633,19 +4478,19 @@
         <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D11" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -4653,7 +4498,7 @@
         <v>352</v>
       </c>
       <c r="B12" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C12" t="s">
         <v>352</v>
@@ -4665,7 +4510,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -4673,7 +4518,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -4682,15 +4527,15 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B14" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -4702,7 +4547,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -4710,7 +4555,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -4727,10 +4572,10 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B16" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -4739,7 +4584,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -4747,7 +4592,7 @@
         <v>348</v>
       </c>
       <c r="B17" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -4759,24 +4604,24 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
+        <v>356</v>
+      </c>
+      <c r="B18" t="s">
+        <v>549</v>
+      </c>
+      <c r="C18" t="s">
         <v>357</v>
-      </c>
-      <c r="B18" t="s">
-        <v>551</v>
-      </c>
-      <c r="C18" t="s">
-        <v>358</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -4784,19 +4629,19 @@
         <v>353</v>
       </c>
       <c r="B19" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D19" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -4804,39 +4649,39 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D20" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B21" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -4844,7 +4689,7 @@
         <v>348</v>
       </c>
       <c r="B22" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -4856,7 +4701,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -4864,19 +4709,19 @@
         <v>347</v>
       </c>
       <c r="B23" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C23" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D23" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -4884,19 +4729,19 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C24" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D24" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -4904,7 +4749,7 @@
         <v>354</v>
       </c>
       <c r="B25" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -4913,7 +4758,7 @@
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -4921,7 +4766,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -4930,7 +4775,7 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -4938,7 +4783,7 @@
         <v>355</v>
       </c>
       <c r="B27" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
@@ -4947,15 +4792,15 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>356</v>
+        <v>569</v>
       </c>
       <c r="B28" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
@@ -4964,15 +4809,15 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B29" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
@@ -4984,15 +4829,15 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B30" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
@@ -5001,15 +4846,15 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B31" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -5018,15 +4863,15 @@
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B32" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
@@ -5035,35 +4880,35 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
+        <v>407</v>
+      </c>
+      <c r="B33" t="s">
+        <v>551</v>
+      </c>
+      <c r="C33" t="s">
+        <v>358</v>
+      </c>
+      <c r="D33" t="s">
+        <v>553</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
         <v>408</v>
-      </c>
-      <c r="B33" t="s">
-        <v>553</v>
-      </c>
-      <c r="C33" t="s">
-        <v>359</v>
-      </c>
-      <c r="D33" t="s">
-        <v>555</v>
-      </c>
-      <c r="F33" t="b">
-        <v>1</v>
-      </c>
-      <c r="G33" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B34" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C34" t="s">
         <v>18</v>
@@ -5075,35 +4920,35 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B35" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B36" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
@@ -5115,15 +4960,15 @@
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B37" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
@@ -5132,15 +4977,15 @@
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B38" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
@@ -5149,7 +4994,7 @@
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -5157,7 +5002,7 @@
         <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
@@ -5166,15 +5011,15 @@
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B40" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
@@ -5183,15 +5028,15 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>414</v>
+        <v>570</v>
       </c>
       <c r="B41" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
@@ -5200,7 +5045,7 @@
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -5208,24 +5053,24 @@
         <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G42" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B43" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C43" t="s">
         <v>18</v>
@@ -5234,15 +5079,15 @@
         <v>1</v>
       </c>
       <c r="G43" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B44" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C44" t="s">
         <v>18</v>
@@ -5254,35 +5099,35 @@
         <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B45" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C45" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D45" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
       </c>
       <c r="G45" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B46" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C46" t="s">
         <v>18</v>
@@ -5294,15 +5139,15 @@
         <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B47" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C47" t="s">
         <v>18</v>
@@ -5311,15 +5156,15 @@
         <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B48" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C48" t="s">
         <v>18</v>
@@ -5328,7 +5173,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -5336,7 +5181,7 @@
         <v>26</v>
       </c>
       <c r="B49" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C49" t="s">
         <v>18</v>
@@ -5345,7 +5190,7 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -5353,7 +5198,7 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C50" t="s">
         <v>18</v>
@@ -5362,15 +5207,15 @@
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B51" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C51" t="s">
         <v>18</v>
@@ -5379,15 +5224,15 @@
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B52" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C52" t="s">
         <v>18</v>
@@ -5399,35 +5244,35 @@
         <v>0</v>
       </c>
       <c r="G52" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B53" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C53" t="s">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="F53" t="b">
         <v>0</v>
       </c>
       <c r="G53" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B54" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C54" t="s">
         <v>17</v>
@@ -5439,35 +5284,35 @@
         <v>0</v>
       </c>
       <c r="G54" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B55" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C55" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D55" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
       </c>
       <c r="G55" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B56" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C56" t="s">
         <v>18</v>
@@ -5479,15 +5324,15 @@
         <v>0</v>
       </c>
       <c r="G56" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B57" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C57" t="s">
         <v>18</v>
@@ -5496,15 +5341,15 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B58" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C58" t="s">
         <v>18</v>
@@ -5513,7 +5358,7 @@
         <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -5521,7 +5366,7 @@
         <v>26</v>
       </c>
       <c r="B59" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C59" t="s">
         <v>18</v>
@@ -5530,7 +5375,7 @@
         <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -5538,7 +5383,7 @@
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C60" t="s">
         <v>18</v>
@@ -5547,7 +5392,7 @@
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="I60" t="b">
         <v>1</v>
@@ -5558,30 +5403,30 @@
         <v>24</v>
       </c>
       <c r="B61" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C61" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D61" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F61" t="b">
         <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B62" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E62" t="b">
         <v>1</v>
@@ -5590,66 +5435,66 @@
         <v>0</v>
       </c>
       <c r="G62" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B63" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C63" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F63" t="b">
         <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B64" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C64" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F64" t="b">
         <v>1</v>
       </c>
       <c r="G64" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B65" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C65" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F65" t="b">
         <v>1</v>
       </c>
       <c r="G65" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B66" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C66" t="s">
         <v>18</v>
@@ -5661,35 +5506,35 @@
         <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B67" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F67" t="b">
         <v>0</v>
       </c>
       <c r="G67" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B68" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C68" t="s">
         <v>17</v>
@@ -5701,35 +5546,35 @@
         <v>0</v>
       </c>
       <c r="G68" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B69" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C69" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D69" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F69" t="b">
         <v>0</v>
       </c>
       <c r="G69" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B70" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C70" t="s">
         <v>18</v>
@@ -5741,15 +5586,15 @@
         <v>0</v>
       </c>
       <c r="G70" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B71" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C71" t="s">
         <v>18</v>
@@ -5758,15 +5603,15 @@
         <v>1</v>
       </c>
       <c r="G71" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B72" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C72" t="s">
         <v>18</v>
@@ -5775,7 +5620,7 @@
         <v>1</v>
       </c>
       <c r="G72" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -5783,7 +5628,7 @@
         <v>26</v>
       </c>
       <c r="B73" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C73" t="s">
         <v>18</v>
@@ -5792,7 +5637,7 @@
         <v>1</v>
       </c>
       <c r="G73" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -5800,7 +5645,7 @@
         <v>6</v>
       </c>
       <c r="B74" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C74" t="s">
         <v>18</v>
@@ -5809,7 +5654,7 @@
         <v>1</v>
       </c>
       <c r="G74" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="I74" t="b">
         <v>1</v>
@@ -5817,30 +5662,30 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B75" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C75" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D75" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F75" t="b">
         <v>1</v>
       </c>
       <c r="G75" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B76" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C76" t="s">
         <v>18</v>
@@ -5852,7 +5697,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -5860,13 +5705,13 @@
         <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F77" t="b">
         <v>1</v>
       </c>
       <c r="G77" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -5874,64 +5719,64 @@
         <v>24</v>
       </c>
       <c r="B78" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F78" t="b">
         <v>0</v>
       </c>
       <c r="G78" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B79" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F79" t="b">
         <v>0</v>
       </c>
       <c r="G79" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B80" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C80" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F80" t="b">
         <v>1</v>
       </c>
       <c r="G80" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="81" spans="1:14">
       <c r="A81" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B81" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C81" t="s">
         <v>18</v>
@@ -5940,72 +5785,72 @@
         <v>1</v>
       </c>
       <c r="G81" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="82" spans="1:14">
       <c r="A82" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B82" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C82" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F82" t="b">
         <v>1</v>
       </c>
       <c r="G82" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="83" spans="1:14">
       <c r="A83" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B83" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C83" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F83" t="b">
         <v>1</v>
       </c>
       <c r="G83" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="N83" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="84" spans="1:14">
       <c r="A84" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B84" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C84" t="s">
+        <v>458</v>
+      </c>
+      <c r="F84" t="b">
+        <v>1</v>
+      </c>
+      <c r="G84" t="s">
+        <v>463</v>
+      </c>
+      <c r="N84" t="s">
         <v>460</v>
-      </c>
-      <c r="F84" t="b">
-        <v>1</v>
-      </c>
-      <c r="G84" t="s">
-        <v>465</v>
-      </c>
-      <c r="N84" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="85" spans="1:14">
       <c r="A85" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B85" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C85" t="s">
         <v>18</v>
@@ -6014,15 +5859,15 @@
         <v>1</v>
       </c>
       <c r="G85" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="86" spans="1:14">
       <c r="A86" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B86" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C86" t="s">
         <v>17</v>
@@ -6031,35 +5876,35 @@
         <v>1</v>
       </c>
       <c r="G86" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="87" spans="1:14">
       <c r="A87" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B87" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C87" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D87" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F87" t="b">
         <v>1</v>
       </c>
       <c r="G87" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="88" spans="1:14">
       <c r="A88" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B88" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C88" t="s">
         <v>18</v>
@@ -6071,15 +5916,15 @@
         <v>0</v>
       </c>
       <c r="G88" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="89" spans="1:14">
       <c r="A89" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B89" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C89" t="s">
         <v>18</v>
@@ -6088,15 +5933,15 @@
         <v>1</v>
       </c>
       <c r="G89" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="90" spans="1:14">
       <c r="A90" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B90" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C90" t="s">
         <v>18</v>
@@ -6105,15 +5950,15 @@
         <v>1</v>
       </c>
       <c r="G90" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="91" spans="1:14">
       <c r="A91" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B91" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C91" t="s">
         <v>18</v>
@@ -6122,15 +5967,15 @@
         <v>1</v>
       </c>
       <c r="G91" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="92" spans="1:14">
       <c r="A92" t="s">
-        <v>414</v>
+        <v>570</v>
       </c>
       <c r="B92" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C92" t="s">
         <v>18</v>
@@ -6139,15 +5984,15 @@
         <v>1</v>
       </c>
       <c r="G92" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="93" spans="1:14">
       <c r="A93" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B93" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C93" t="s">
         <v>18</v>
@@ -6156,15 +6001,15 @@
         <v>1</v>
       </c>
       <c r="G93" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="94" spans="1:14">
       <c r="A94" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B94" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C94" t="s">
         <v>18</v>
@@ -6173,7 +6018,7 @@
         <v>1</v>
       </c>
       <c r="G94" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I94" t="b">
         <v>1</v>
@@ -6181,10 +6026,10 @@
     </row>
     <row r="95" spans="1:14">
       <c r="A95" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B95" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C95" t="s">
         <v>18</v>
@@ -6196,15 +6041,15 @@
         <v>0</v>
       </c>
       <c r="G95" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="96" spans="1:14">
       <c r="A96" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B96" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C96" t="s">
         <v>18</v>
@@ -6213,15 +6058,15 @@
         <v>1</v>
       </c>
       <c r="G96" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B97" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C97" t="s">
         <v>18</v>
@@ -6230,15 +6075,15 @@
         <v>1</v>
       </c>
       <c r="G97" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B98" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C98" t="s">
         <v>18</v>
@@ -6250,15 +6095,15 @@
         <v>0</v>
       </c>
       <c r="G98" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B99" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C99" t="s">
         <v>18</v>
@@ -6267,15 +6112,15 @@
         <v>0</v>
       </c>
       <c r="G99" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B100" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C100" t="s">
         <v>18</v>
@@ -6284,18 +6129,18 @@
         <v>0</v>
       </c>
       <c r="G100" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B101" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C101" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E101" t="b">
         <v>1</v>
@@ -6304,15 +6149,15 @@
         <v>0</v>
       </c>
       <c r="G101" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B102" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C102" t="s">
         <v>18</v>
@@ -6321,15 +6166,15 @@
         <v>1</v>
       </c>
       <c r="G102" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B103" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C103" t="s">
         <v>18</v>
@@ -6341,255 +6186,255 @@
         <v>0</v>
       </c>
       <c r="G103" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B104" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C104" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F104" t="b">
         <v>1</v>
       </c>
       <c r="G104" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="C1 C3:C5 C7 A27:H27 E24:H24 A13:H15 A29:A32 G29 C29:C32 A25:E26 G25:H26 A28:E28 G28:H28 B34:B35 C36:C67 C70:C90 C94:C1048576">
-    <cfRule type="cellIs" dxfId="61" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="56" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="60" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="54" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="59" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="52" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C10">
-    <cfRule type="cellIs" dxfId="58" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="51" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:C20">
-    <cfRule type="cellIs" dxfId="57" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="50" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11 C17:C18">
-    <cfRule type="cellIs" dxfId="56" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="49" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="55" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="48" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="54" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="47" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="53" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C12 C17:C21 A27:H27 E24:H24 A13:H15 A29:A32 G29 C29:C32 A25:E26 G25:H26 A28:E28 G28:H28 B34:B35 C36:C67 C70:C90 C94:C1048576">
-    <cfRule type="cellIs" dxfId="52" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:E22 G22:H23 A23:C24 E23">
-    <cfRule type="cellIs" dxfId="51" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:E22 G22:H23 A23:C24 E23">
-    <cfRule type="cellIs" dxfId="50" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="42" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="49" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="41" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="48" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:B16 F16:G16">
-    <cfRule type="cellIs" dxfId="47" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="39" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:B16 F16:G16">
-    <cfRule type="cellIs" dxfId="46" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="38" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35 C35 A34 C34:D34 F34:H34">
-    <cfRule type="cellIs" dxfId="45" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="37" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35 C35 A34 C34:D34 F34:H34">
-    <cfRule type="cellIs" dxfId="44" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="43" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="35" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="42" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="cellIs" dxfId="41" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="33" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="cellIs" dxfId="40" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="32" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="39" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="38" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="30" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44">
-    <cfRule type="cellIs" dxfId="37" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="29" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44">
-    <cfRule type="cellIs" dxfId="36" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="28" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="cellIs" dxfId="35" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="cellIs" dxfId="34" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G66">
-    <cfRule type="cellIs" dxfId="33" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G66">
-    <cfRule type="cellIs" dxfId="32" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="cellIs" dxfId="31" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69">
-    <cfRule type="cellIs" dxfId="29" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69">
-    <cfRule type="cellIs" dxfId="28" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76:B87">
-    <cfRule type="cellIs" dxfId="27" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76:B87">
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91:C93">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91:C93">
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"mref"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6612,9 +6457,9 @@
       <selection activeCell="A303" sqref="A303:XFD303"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -8144,9 +7989,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -8248,89 +8093,89 @@
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>522</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>529</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>529</v>
+      </c>
+      <c r="B3" t="s">
+        <v>530</v>
+      </c>
+      <c r="C3" t="s">
+        <v>530</v>
+      </c>
+      <c r="D3" t="s">
         <v>531</v>
       </c>
-      <c r="B3" t="s">
-        <v>532</v>
-      </c>
-      <c r="C3" t="s">
-        <v>532</v>
-      </c>
-      <c r="D3" t="s">
-        <v>533</v>
-      </c>
       <c r="E3" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B4" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C4" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D4" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
   </sheetData>

</xml_diff>